<commit_message>
Updated the results spreadsheet with an accurate Kakuro experiment
</commit_message>
<xml_diff>
--- a/ResultsSummary.xlsx
+++ b/ResultsSummary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rh347/SideProjects/puzsmt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018EAB01-7D36-8C40-B8C4-82923B65B18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B1544-1AC2-AE47-82A4-3D7DD2ABD1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{2F2E770E-C311-CD46-AEFE-0C515743FDD9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Sudoku &amp; Variants</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">We define an instance/example as stoopid if there are other cells that are obviously going to be solved by hand/computer </t>
+  </si>
+  <si>
+    <t>step 7 is done by us way earlier, step 8 is a MUS of size 8, step 9 and 10 we find simpler/other deductions first that leave these as super easy deductions.</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48B92C3-9987-254F-BC13-341E55514592}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,7 +533,7 @@
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -547,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -558,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -575,7 +578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -589,7 +592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -606,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -620,7 +623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -637,7 +640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -651,18 +654,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
       <c r="D9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -676,7 +685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -693,7 +702,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -701,7 +710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -718,7 +727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -732,7 +741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -746,7 +755,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>30</v>
       </c>

</xml_diff>